<commit_message>
update: module_list in xlsx
</commit_message>
<xml_diff>
--- a/assets/1.Module_list/Module_list_ir.module.module.xlsx
+++ b/assets/1.Module_list/Module_list_ir.module.module.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="62">
   <si>
     <t>Module Name</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>16.0.1.2</t>
+  </si>
+  <si>
+    <t>grading_template</t>
   </si>
   <si>
     <t>In-App Purchases</t>
@@ -540,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -748,7 +751,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
@@ -774,11 +777,13 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>
@@ -786,14 +791,14 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
@@ -804,13 +809,11 @@
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
@@ -818,13 +821,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>24</v>
@@ -835,16 +838,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>9</v>
@@ -855,13 +858,13 @@
         <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>9</v>
@@ -872,7 +875,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -886,14 +889,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>9</v>
@@ -901,14 +906,14 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>9</v>
@@ -919,11 +924,11 @@
         <v>45</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>9</v>
@@ -934,7 +939,7 @@
         <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -949,13 +954,11 @@
         <v>47</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>9</v>
@@ -966,11 +969,13 @@
         <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D27" s="2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>9</v>
@@ -978,14 +983,14 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>9</v>
@@ -993,14 +998,14 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>9</v>
@@ -1011,13 +1016,11 @@
         <v>53</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>9</v>
@@ -1028,11 +1031,13 @@
         <v>54</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>9</v>
@@ -1077,7 +1082,7 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>9</v>
@@ -1092,7 +1097,7 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>9</v>
@@ -1107,9 +1112,24 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1119,13 +1139,14 @@
     <hyperlink ref="C11" r:id="rId2"/>
     <hyperlink ref="C12" r:id="rId3"/>
     <hyperlink ref="C13" r:id="rId4"/>
-    <hyperlink ref="C17" r:id="rId5"/>
+    <hyperlink ref="C15" r:id="rId5"/>
     <hyperlink ref="C18" r:id="rId6"/>
     <hyperlink ref="C19" r:id="rId7"/>
     <hyperlink ref="C20" r:id="rId8"/>
     <hyperlink ref="C21" r:id="rId9"/>
-    <hyperlink ref="C26" r:id="rId10"/>
-    <hyperlink ref="C30" r:id="rId11"/>
+    <hyperlink ref="C22" r:id="rId10"/>
+    <hyperlink ref="C27" r:id="rId11"/>
+    <hyperlink ref="C31" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: update module-list and project_grading
</commit_message>
<xml_diff>
--- a/assets/1.Module_list/Module_list_ir.module.module.xlsx
+++ b/assets/1.Module_list/Module_list_ir.module.module.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
   <si>
     <t>Module Name</t>
   </si>
@@ -91,12 +91,18 @@
     <t>16.0.0.1</t>
   </si>
   <si>
+    <t>Custom Form View</t>
+  </si>
+  <si>
+    <t>My Company</t>
+  </si>
+  <si>
+    <t>Custom List View</t>
+  </si>
+  <si>
     <t>email_server_config</t>
   </si>
   <si>
-    <t>My Company</t>
-  </si>
-  <si>
     <t>Feedback Ticket Management</t>
   </si>
   <si>
@@ -106,7 +112,7 @@
     <t>16.0.1.2</t>
   </si>
   <si>
-    <t>grading_template</t>
+    <t>Funix Learning ProjectGrading Template</t>
   </si>
   <si>
     <t>In-App Purchases</t>
@@ -118,12 +124,6 @@
     <t>IAP / Mail</t>
   </si>
   <si>
-    <t>Learning Program</t>
-  </si>
-  <si>
-    <t>funix</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Partner Autocomplete</t>
+  </si>
+  <si>
+    <t>portal_common</t>
   </si>
   <si>
     <t>Portal Student Management</t>
@@ -543,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -751,7 +754,7 @@
         <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
@@ -762,11 +765,13 @@
         <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>9</v>
@@ -774,7 +779,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>26</v>
@@ -791,14 +796,14 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
@@ -806,14 +811,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
@@ -821,16 +828,14 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
@@ -838,16 +843,14 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>9</v>
@@ -855,16 +858,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>9</v>
@@ -872,16 +875,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>9</v>
@@ -889,10 +892,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -906,14 +909,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>9</v>
@@ -921,14 +926,14 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>9</v>
@@ -936,14 +941,14 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>9</v>
@@ -951,14 +956,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>9</v>
@@ -966,16 +973,14 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>9</v>
@@ -983,14 +988,14 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>9</v>
@@ -998,14 +1003,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D29" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>9</v>
@@ -1013,14 +1020,14 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>9</v>
@@ -1028,16 +1035,14 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>9</v>
@@ -1045,7 +1050,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
@@ -1060,14 +1065,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="D33" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>9</v>
@@ -1075,7 +1082,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>6</v>
@@ -1090,14 +1097,14 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>9</v>
@@ -1105,14 +1112,14 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>9</v>
@@ -1120,16 +1127,46 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="B39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1139,14 +1176,16 @@
     <hyperlink ref="C11" r:id="rId2"/>
     <hyperlink ref="C12" r:id="rId3"/>
     <hyperlink ref="C13" r:id="rId4"/>
-    <hyperlink ref="C15" r:id="rId5"/>
-    <hyperlink ref="C18" r:id="rId6"/>
-    <hyperlink ref="C19" r:id="rId7"/>
+    <hyperlink ref="C14" r:id="rId5"/>
+    <hyperlink ref="C15" r:id="rId6"/>
+    <hyperlink ref="C17" r:id="rId7"/>
     <hyperlink ref="C20" r:id="rId8"/>
     <hyperlink ref="C21" r:id="rId9"/>
     <hyperlink ref="C22" r:id="rId10"/>
-    <hyperlink ref="C27" r:id="rId11"/>
-    <hyperlink ref="C31" r:id="rId12"/>
+    <hyperlink ref="C23" r:id="rId11"/>
+    <hyperlink ref="C26" r:id="rId12"/>
+    <hyperlink ref="C29" r:id="rId13"/>
+    <hyperlink ref="C33" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>